<commit_message>
mettre à jour scrum v0.2
Signed-off-by: Tristan Charpentier <tristan_charpentier@hotmail.com>
</commit_message>
<xml_diff>
--- a/scrum/scrum_product_backlog.xlsx
+++ b/scrum/scrum_product_backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Documents/L2/013/ForestWorld/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Documents/L2/013/ForestWorld/scrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01BA335-3084-AC4E-9617-A5ABBD1B54E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C57321D-E7C0-A442-B6C3-FED1D19B2C2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16940" xr2:uid="{25DF086B-56B6-E348-8940-5B61FC8CF5A8}"/>
   </bookViews>
@@ -354,61 +354,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightGray">
-          <fgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightGray">
-          <fgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -759,7 +705,7 @@
   <dimension ref="A1:AJ151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="A1:G9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,10 +750,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="20"/>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="22"/>
       <c r="H2" s="12"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -849,11 +795,11 @@
       <c r="D3" s="28">
         <v>2</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="23"/>
       <c r="H3" s="14"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -895,10 +841,10 @@
       <c r="D4" s="28">
         <v>3</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="21"/>
+      <c r="F4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="15"/>
       <c r="G4" s="23"/>
       <c r="H4" s="14"/>
       <c r="I4" s="2"/>
@@ -6460,17 +6406,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",G1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>